<commit_message>
commit fixed and reformatted Afghanistan data
</commit_message>
<xml_diff>
--- a/Afghanistan_Raw.xlsx
+++ b/Afghanistan_Raw.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hilgert\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iandr\KEYS_Training\Data\Data_Workfolder\KEYS_Training_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5E90CA-FFD4-41AD-ACDC-D25AAA12A415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Afghanistan_Raw.cc" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t>country</t>
   </si>
@@ -55,12 +56,21 @@
   </si>
   <si>
     <t>Do we need more data?</t>
+  </si>
+  <si>
+    <t>Notes/Comments</t>
+  </si>
+  <si>
+    <t>no continent in orginal data, just 'tbd'</t>
+  </si>
+  <si>
+    <t>no year in original data, just 'n/a'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -860,16 +870,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -888,8 +904,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -909,7 +928,7 @@
         <v>635.34135100000003</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -929,7 +948,7 @@
         <v>726.73405479999997</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -949,7 +968,7 @@
         <v>974.58033839999996</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -968,8 +987,11 @@
       <c r="F5">
         <v>779.44531449999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -989,7 +1011,7 @@
         <v>820.85302960000001</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1009,7 +1031,7 @@
         <v>853.10071000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1029,7 +1051,7 @@
         <v>836.19713820000004</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1049,7 +1071,7 @@
         <v>739.98110580000002</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1069,7 +1091,7 @@
         <v>786.11335999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1088,8 +1110,11 @@
       <c r="F11">
         <v>978.01143879999995</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1109,7 +1134,7 @@
         <v>852.39594480000005</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1129,8 +1154,8 @@
         <v>649.34139519999997</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>